<commit_message>
updated ClueLayout.xlsx, changed color of center and title squares
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenda\CSCI306\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carso\eclipse-workspace\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D211CE-6373-4213-8ECB-95256400CB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B897D26-6D95-4D28-A504-417E1C0022F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F141023-AB6C-4FB6-8629-EA7309D3762D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F141023-AB6C-4FB6-8629-EA7309D3762D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +202,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -215,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -224,6 +230,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,12 +549,12 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -605,7 +613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -636,7 +644,7 @@
       <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -667,14 +675,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -698,7 +706,7 @@
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -722,21 +730,21 @@
       <c r="R3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="S3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -784,14 +792,14 @@
       <c r="R4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -853,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -915,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -977,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1039,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1101,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1163,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1206,7 +1214,7 @@
       <c r="N11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="8" t="s">
         <v>20</v>
       </c>
       <c r="P11" s="2" t="s">
@@ -1225,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1247,7 +1255,7 @@
       <c r="G12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1268,7 +1276,7 @@
       <c r="N12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="8" t="s">
         <v>21</v>
       </c>
       <c r="P12" s="2" t="s">
@@ -1287,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1309,7 +1317,7 @@
       <c r="G13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1349,7 +1357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1411,7 +1419,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1473,7 +1481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1535,7 +1543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1597,7 +1605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1659,7 +1667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1721,7 +1729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1752,7 +1760,7 @@
       <c r="J20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="8" t="s">
         <v>35</v>
       </c>
       <c r="L20" s="2" t="s">
@@ -1783,7 +1791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1814,7 +1822,7 @@
       <c r="J21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L21" s="2" t="s">
@@ -1845,7 +1853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1900,14 +1908,14 @@
       <c r="R22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="S22" s="8" t="s">
         <v>33</v>
       </c>
       <c r="T22" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1965,15 +1973,15 @@
       <c r="S23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="T23" s="2" t="s">
+      <c r="T23" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -2031,11 +2039,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -2093,7 +2101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2155,7 +2163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2217,7 +2225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2279,7 +2287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2310,7 +2318,7 @@
       <c r="J29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" s="8" t="s">
         <v>26</v>
       </c>
       <c r="L29" s="2" t="s">
@@ -2341,7 +2349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2372,7 +2380,7 @@
       <c r="J30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="8" t="s">
         <v>27</v>
       </c>
       <c r="L30" s="2" t="s">
@@ -2403,7 +2411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>

</xml_diff>